<commit_message>
capture tests fixed, goBoard finds captures
- invalid tests had to be fixed
- capture recognition algorithm fixed
- all tests pass!
</commit_message>
<xml_diff>
--- a/StrategyMaster2013/src/game/go/capture_configurations.xlsx
+++ b/StrategyMaster2013/src/game/go/capture_configurations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="7" r:id="rId1"/>
@@ -12,14 +12,18 @@
     <sheet name="Edges" sheetId="6" r:id="rId3"/>
     <sheet name="Center" sheetId="8" r:id="rId4"/>
     <sheet name="Complex" sheetId="9" r:id="rId5"/>
+    <sheet name="MultiCapture)" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="asdfa">#REF!</definedName>
     <definedName name="BoardSize" localSheetId="3">Center!#REF!</definedName>
     <definedName name="BoardSize" localSheetId="4">Complex!#REF!</definedName>
     <definedName name="BoardSize" localSheetId="1">Corners!$A$2</definedName>
     <definedName name="BoardSize" localSheetId="2">Edges!#REF!</definedName>
+    <definedName name="BoardSize" localSheetId="5">'MultiCapture)'!#REF!</definedName>
     <definedName name="BoardSize" localSheetId="0">template!#REF!</definedName>
     <definedName name="BoardSize">#REF!</definedName>
+    <definedName name="vb" localSheetId="5">#REF!</definedName>
     <definedName name="vb">#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="13">
   <si>
     <t>w</t>
   </si>
@@ -57,6 +61,15 @@
   </si>
   <si>
     <t>b2d</t>
+  </si>
+  <si>
+    <t>b23</t>
+  </si>
+  <si>
+    <t>b22</t>
+  </si>
+  <si>
+    <t>b24</t>
   </si>
 </sst>
 </file>
@@ -182,7 +195,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="34">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2917,28 +2972,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5213,18 +5268,18 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="30" priority="2" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7530,28 +7585,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9867,28 +9922,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9901,7 +9956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="AC31" sqref="AC31"/>
     </sheetView>
   </sheetViews>
@@ -12248,6 +12303,2333 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="w">
+      <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:AN21">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="w">
+      <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:AN23 A1:U2">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="b2">
+      <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO3:AO21">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="b2">
+      <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AO24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AE25" sqref="AE25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" style="5"/>
+    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" customWidth="1"/>
+    <col min="21" max="21" width="4.7109375" style="10"/>
+    <col min="22" max="40" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="V1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+    </row>
+    <row r="2" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+    </row>
+    <row r="3" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="5">
+        <v>18</v>
+      </c>
+      <c r="V3" s="4" t="str">
+        <f>IF(ISNUMBER(SEARCH("b",B3)),CONCATENATE(B3,": ",V$22,", ",$U3,),IF(ISNUMBER(SEARCH("w",B3)),CONCATENATE(B3,": ",V$22,", ",$U3,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W3" s="4" t="str">
+        <f t="shared" ref="W3:AL18" si="0">IF(ISNUMBER(SEARCH("b",C3)),CONCATENATE(C3,": ",W$22,", ",$U3,),IF(ISNUMBER(SEARCH("w",C3)),CONCATENATE(C3,": ",W$22,", ",$U3,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM3" s="4" t="str">
+        <f t="shared" ref="AM3:AN18" si="1">IF(ISNUMBER(SEARCH("b",S3)),CONCATENATE(S3,": ",AM$22,", ",$U3,),IF(ISNUMBER(SEARCH("w",S3)),CONCATENATE(S3,": ",AM$22,", ",$U3,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN3" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO3" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="5">
+        <v>17</v>
+      </c>
+      <c r="V4" s="4" t="str">
+        <f t="shared" ref="V4:AK21" si="2">IF(ISNUMBER(SEARCH("b",B4)),CONCATENATE(B4,": ",V$22,", ",$U4,),IF(ISNUMBER(SEARCH("w",B4)),CONCATENATE(B4,": ",V$22,", ",$U4,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM4" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN4" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO4" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="5">
+        <v>16</v>
+      </c>
+      <c r="V5" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO5" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="5">
+        <v>15</v>
+      </c>
+      <c r="V6" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO6" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="5">
+        <v>14</v>
+      </c>
+      <c r="V7" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO7" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="5">
+        <v>13</v>
+      </c>
+      <c r="V8" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO8" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="5">
+        <v>12</v>
+      </c>
+      <c r="V9" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 10, 12</v>
+      </c>
+      <c r="AG9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO9" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="5">
+        <v>11</v>
+      </c>
+      <c r="V10" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 9, 11</v>
+      </c>
+      <c r="AF10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 10, 11</v>
+      </c>
+      <c r="AG10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b22: 11, 11</v>
+      </c>
+      <c r="AH10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO10" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="5">
+        <v>10</v>
+      </c>
+      <c r="V11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 8, 10</v>
+      </c>
+      <c r="AE11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 9, 10</v>
+      </c>
+      <c r="AF11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 10, 10</v>
+      </c>
+      <c r="AG11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 11, 10</v>
+      </c>
+      <c r="AH11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 12, 10</v>
+      </c>
+      <c r="AI11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO11" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="5">
+        <v>9</v>
+      </c>
+      <c r="V12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 7, 9</v>
+      </c>
+      <c r="AD12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 8, 9</v>
+      </c>
+      <c r="AE12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b24: 9, 9</v>
+      </c>
+      <c r="AF12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 10, 9</v>
+      </c>
+      <c r="AG12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 11, 9</v>
+      </c>
+      <c r="AH12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO12" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="5">
+        <v>8</v>
+      </c>
+      <c r="V13" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 8, 8</v>
+      </c>
+      <c r="AE13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 9, 8</v>
+      </c>
+      <c r="AF13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 10, 8</v>
+      </c>
+      <c r="AG13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 11, 8</v>
+      </c>
+      <c r="AH13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 12, 8</v>
+      </c>
+      <c r="AI13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO13" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="5">
+        <v>7</v>
+      </c>
+      <c r="V14" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 9, 7</v>
+      </c>
+      <c r="AF14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 10, 7</v>
+      </c>
+      <c r="AG14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b23: 11, 7</v>
+      </c>
+      <c r="AH14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 12, 7</v>
+      </c>
+      <c r="AI14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 13, 7</v>
+      </c>
+      <c r="AJ14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO14" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="5">
+        <v>6</v>
+      </c>
+      <c r="V15" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 10, 6</v>
+      </c>
+      <c r="AG15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 12, 6</v>
+      </c>
+      <c r="AI15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO15" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="5">
+        <v>5</v>
+      </c>
+      <c r="V16" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO16" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="5">
+        <v>4</v>
+      </c>
+      <c r="V17" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO17" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="5">
+        <v>3</v>
+      </c>
+      <c r="V18" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL18" s="4" t="str">
+        <f t="shared" ref="AL18:AN22" si="3">IF(ISNUMBER(SEARCH("b",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,),IF(ISNUMBER(SEARCH("w",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="5">
+        <v>2</v>
+      </c>
+      <c r="V19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO19" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="5">
+        <v>1</v>
+      </c>
+      <c r="V20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="5">
+        <v>0</v>
+      </c>
+      <c r="V21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" s="5" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2</v>
+      </c>
+      <c r="E22" s="5">
+        <v>3</v>
+      </c>
+      <c r="F22" s="5">
+        <v>4</v>
+      </c>
+      <c r="G22" s="5">
+        <v>5</v>
+      </c>
+      <c r="H22" s="5">
+        <v>6</v>
+      </c>
+      <c r="I22" s="5">
+        <v>7</v>
+      </c>
+      <c r="J22" s="5">
+        <v>8</v>
+      </c>
+      <c r="K22" s="5">
+        <v>9</v>
+      </c>
+      <c r="L22" s="5">
+        <v>10</v>
+      </c>
+      <c r="M22" s="5">
+        <v>11</v>
+      </c>
+      <c r="N22" s="5">
+        <v>12</v>
+      </c>
+      <c r="O22" s="5">
+        <v>13</v>
+      </c>
+      <c r="P22" s="5">
+        <v>14</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>15</v>
+      </c>
+      <c r="R22" s="5">
+        <v>16</v>
+      </c>
+      <c r="S22" s="5">
+        <v>17</v>
+      </c>
+      <c r="T22" s="5">
+        <v>18</v>
+      </c>
+      <c r="V22" s="5">
+        <v>0</v>
+      </c>
+      <c r="W22" s="5">
+        <v>1</v>
+      </c>
+      <c r="X22" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y22" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z22" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA22" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB22" s="5">
+        <v>6</v>
+      </c>
+      <c r="AC22" s="5">
+        <v>7</v>
+      </c>
+      <c r="AD22" s="5">
+        <v>8</v>
+      </c>
+      <c r="AE22" s="5">
+        <v>9</v>
+      </c>
+      <c r="AF22" s="5">
+        <v>10</v>
+      </c>
+      <c r="AG22" s="5">
+        <v>11</v>
+      </c>
+      <c r="AH22" s="5">
+        <v>12</v>
+      </c>
+      <c r="AI22" s="5">
+        <v>13</v>
+      </c>
+      <c r="AJ22" s="5">
+        <v>14</v>
+      </c>
+      <c r="AK22" s="5">
+        <v>15</v>
+      </c>
+      <c r="AL22" s="5">
+        <v>16</v>
+      </c>
+      <c r="AM22" s="5">
+        <v>17</v>
+      </c>
+      <c r="AN22" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:T2"/>
+    <mergeCell ref="V1:AN2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:T21">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
another test and capture recognition still works
</commit_message>
<xml_diff>
--- a/StrategyMaster2013/src/game/go/capture_configurations.xlsx
+++ b/StrategyMaster2013/src/game/go/capture_configurations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="7" r:id="rId1"/>
@@ -12,17 +12,21 @@
     <sheet name="Edges" sheetId="6" r:id="rId3"/>
     <sheet name="Center" sheetId="8" r:id="rId4"/>
     <sheet name="Complex" sheetId="9" r:id="rId5"/>
-    <sheet name="MultiCapture)" sheetId="10" r:id="rId6"/>
+    <sheet name="MultiCapture" sheetId="10" r:id="rId6"/>
+    <sheet name="MoreComplex" sheetId="11" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="asdfa" localSheetId="6">#REF!</definedName>
     <definedName name="asdfa">#REF!</definedName>
     <definedName name="BoardSize" localSheetId="3">Center!#REF!</definedName>
     <definedName name="BoardSize" localSheetId="4">Complex!#REF!</definedName>
     <definedName name="BoardSize" localSheetId="1">Corners!$A$2</definedName>
     <definedName name="BoardSize" localSheetId="2">Edges!#REF!</definedName>
-    <definedName name="BoardSize" localSheetId="5">'MultiCapture)'!#REF!</definedName>
+    <definedName name="BoardSize" localSheetId="6">MoreComplex!#REF!</definedName>
+    <definedName name="BoardSize" localSheetId="5">MultiCapture!#REF!</definedName>
     <definedName name="BoardSize" localSheetId="0">template!#REF!</definedName>
     <definedName name="BoardSize">#REF!</definedName>
+    <definedName name="vb" localSheetId="6">#REF!</definedName>
     <definedName name="vb" localSheetId="5">#REF!</definedName>
     <definedName name="vb">#REF!</definedName>
   </definedNames>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="11">
   <si>
     <t>w</t>
   </si>
@@ -61,12 +65,6 @@
   </si>
   <si>
     <t>b2d</t>
-  </si>
-  <si>
-    <t>b23</t>
-  </si>
-  <si>
-    <t>b22</t>
   </si>
   <si>
     <t>b24</t>
@@ -178,6 +176,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -190,12 +189,74 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -403,6 +464,48 @@
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -740,93 +843,93 @@
     <col min="1" max="1" width="4.7109375" style="5"/>
     <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" customWidth="1"/>
-    <col min="21" max="21" width="4.7109375" style="10"/>
+    <col min="21" max="21" width="4.7109375" style="6"/>
     <col min="22" max="40" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="V1" s="8" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="V1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
     </row>
     <row r="2" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
     </row>
     <row r="3" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -2509,7 +2612,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="AL18" s="4" t="str">
-        <f t="shared" ref="AL18:AN22" si="3">IF(ISNUMBER(SEARCH("b",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,),IF(ISNUMBER(SEARCH("w",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,)," "))</f>
+        <f t="shared" ref="AL18:AN21" si="3">IF(ISNUMBER(SEARCH("b",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,),IF(ISNUMBER(SEARCH("w",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,)," "))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="AM18" s="4" t="str">
@@ -2972,28 +3075,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="48" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="47" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="46" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="45" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="44" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="43" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3007,7 +3110,7 @@
   <dimension ref="A1:AO24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3019,91 +3122,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="V1" s="8" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="V1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
     </row>
     <row r="2" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>19</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
     </row>
     <row r="3" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -5268,18 +5371,18 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="42" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="41" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="2" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="39" priority="2" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5292,8 +5395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5303,93 +5406,93 @@
     <col min="9" max="9" width="4.42578125" customWidth="1"/>
     <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" customWidth="1"/>
-    <col min="21" max="21" width="4.7109375" style="10"/>
+    <col min="21" max="21" width="4.7109375" style="6"/>
     <col min="22" max="40" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="V1" s="8" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="V1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
     </row>
     <row r="2" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
     </row>
     <row r="3" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -7585,28 +7688,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="37" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="36" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7619,8 +7722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7628,93 +7731,93 @@
     <col min="1" max="1" width="4.7109375" style="5"/>
     <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" customWidth="1"/>
-    <col min="21" max="21" width="4.7109375" style="10"/>
+    <col min="21" max="21" width="4.7109375" style="6"/>
     <col min="22" max="40" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="V1" s="8" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="V1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
     </row>
     <row r="2" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
     </row>
     <row r="3" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -7940,7 +8043,9 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -7988,7 +8093,7 @@
       </c>
       <c r="AD5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>b2: 8, 16</v>
       </c>
       <c r="AE5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8045,11 +8150,15 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="J6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -8092,15 +8201,15 @@
       </c>
       <c r="AC6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>b: 7, 15</v>
       </c>
       <c r="AD6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>b2: 8, 15</v>
+        <v>w: 8, 15</v>
       </c>
       <c r="AE6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>b: 9, 15</v>
       </c>
       <c r="AF6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -8493,7 +8602,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>1</v>
@@ -8546,7 +8655,7 @@
       </c>
       <c r="AD10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>w: 8, 11</v>
+        <v>b: 8, 11</v>
       </c>
       <c r="AE10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9459,7 +9568,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="AL18" s="4" t="str">
-        <f t="shared" ref="AL18:AN22" si="3">IF(ISNUMBER(SEARCH("b",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,),IF(ISNUMBER(SEARCH("w",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,)," "))</f>
+        <f t="shared" ref="AL18:AN21" si="3">IF(ISNUMBER(SEARCH("b",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,),IF(ISNUMBER(SEARCH("w",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,)," "))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="AM18" s="4" t="str">
@@ -9922,28 +10031,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="32" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="31" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="30" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="29" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="28" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9956,8 +10065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="AC31" sqref="AC31"/>
+    <sheetView topLeftCell="T4" workbookViewId="0">
+      <selection activeCell="Z26" sqref="Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9965,93 +10074,93 @@
     <col min="1" max="1" width="4.7109375" style="5"/>
     <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" customWidth="1"/>
-    <col min="21" max="21" width="4.7109375" style="10"/>
+    <col min="21" max="21" width="4.7109375" style="6"/>
     <col min="22" max="40" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="V1" s="8" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="V1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
     </row>
     <row r="2" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
     </row>
     <row r="3" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -11770,7 +11879,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="AL18" s="4" t="str">
-        <f t="shared" ref="AL18:AN22" si="3">IF(ISNUMBER(SEARCH("b",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,),IF(ISNUMBER(SEARCH("w",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,)," "))</f>
+        <f t="shared" ref="AL18:AN21" si="3">IF(ISNUMBER(SEARCH("b",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,),IF(ISNUMBER(SEARCH("w",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,)," "))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="AM18" s="4" t="str">
@@ -12303,28 +12412,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="26" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12337,8 +12446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AE25" sqref="AE25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12346,93 +12455,93 @@
     <col min="1" max="1" width="4.7109375" style="5"/>
     <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" customWidth="1"/>
-    <col min="21" max="21" width="4.7109375" style="10"/>
+    <col min="21" max="21" width="4.7109375" style="6"/>
     <col min="22" max="40" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="V1" s="8" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="V1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
     </row>
     <row r="2" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
     </row>
     <row r="3" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -13084,11 +13193,11 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -13140,7 +13249,7 @@
       </c>
       <c r="AF9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>b: 10, 12</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="AG9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -13148,7 +13257,7 @@
       </c>
       <c r="AH9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>b: 12, 12</v>
       </c>
       <c r="AI9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -13194,14 +13303,16 @@
       <c r="K10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="O10" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -13252,19 +13363,19 @@
       </c>
       <c r="AF10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>w: 10, 11</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="AG10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>b22: 11, 11</v>
+        <v>b2: 11, 11</v>
       </c>
       <c r="AH10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>w: 12, 11</v>
       </c>
       <c r="AI10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>b: 13, 11</v>
       </c>
       <c r="AJ10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -13424,7 +13535,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>0</v>
@@ -13543,12 +13654,8 @@
       <c r="L13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -13604,11 +13711,11 @@
       </c>
       <c r="AG13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>w: 11, 8</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="AH13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>b: 12, 8</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="AI13" s="4" t="str">
         <f t="shared" si="0"/>
@@ -13658,14 +13765,10 @@
         <v>0</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O14" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -13720,15 +13823,15 @@
       </c>
       <c r="AG14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>b23: 11, 7</v>
+        <v>b: 11, 7</v>
       </c>
       <c r="AH14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>w: 12, 7</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="AI14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>b: 13, 7</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="AJ14" s="4" t="str">
         <f t="shared" si="0"/>
@@ -13766,12 +13869,18 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="L15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M15" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="N15" s="1" t="s">
         <v>1</v>
       </c>
@@ -13818,19 +13927,19 @@
       </c>
       <c r="AD15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>b: 8, 6</v>
       </c>
       <c r="AE15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>w: 9, 6</v>
       </c>
       <c r="AF15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>b: 10, 6</v>
+        <v>b2: 10, 6</v>
       </c>
       <c r="AG15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>w: 11, 6</v>
       </c>
       <c r="AH15" s="4" t="str">
         <f t="shared" si="0"/>
@@ -13877,9 +13986,13 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="M16" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -13928,7 +14041,7 @@
       </c>
       <c r="AE16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>b: 9, 5</v>
       </c>
       <c r="AF16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -13936,7 +14049,7 @@
       </c>
       <c r="AG16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>b: 11, 5</v>
       </c>
       <c r="AH16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -14167,7 +14280,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="AL18" s="4" t="str">
-        <f t="shared" ref="AL18:AN22" si="3">IF(ISNUMBER(SEARCH("b",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,),IF(ISNUMBER(SEARCH("w",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,)," "))</f>
+        <f t="shared" ref="AL18:AN21" si="3">IF(ISNUMBER(SEARCH("b",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,),IF(ISNUMBER(SEARCH("w",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,)," "))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="AM18" s="4" t="str">
@@ -14630,28 +14743,2437 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="19" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="b2">
+      <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AO24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" style="5"/>
+    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" customWidth="1"/>
+    <col min="21" max="21" width="4.7109375" style="6"/>
+    <col min="22" max="40" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="V1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+    </row>
+    <row r="2" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
+    </row>
+    <row r="3" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="5">
+        <v>18</v>
+      </c>
+      <c r="V3" s="4" t="str">
+        <f>IF(ISNUMBER(SEARCH("b",B3)),CONCATENATE(B3,": ",V$22,", ",$U3,),IF(ISNUMBER(SEARCH("w",B3)),CONCATENATE(B3,": ",V$22,", ",$U3,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W3" s="4" t="str">
+        <f t="shared" ref="W3:AL18" si="0">IF(ISNUMBER(SEARCH("b",C3)),CONCATENATE(C3,": ",W$22,", ",$U3,),IF(ISNUMBER(SEARCH("w",C3)),CONCATENATE(C3,": ",W$22,", ",$U3,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 18</v>
+      </c>
+      <c r="AK3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 18</v>
+      </c>
+      <c r="AL3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b2: 16, 18</v>
+      </c>
+      <c r="AM3" s="4" t="str">
+        <f t="shared" ref="AM3:AN18" si="1">IF(ISNUMBER(SEARCH("b",S3)),CONCATENATE(S3,": ",AM$22,", ",$U3,),IF(ISNUMBER(SEARCH("w",S3)),CONCATENATE(S3,": ",AM$22,", ",$U3,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN3" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO3" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="5">
+        <v>17</v>
+      </c>
+      <c r="V4" s="4" t="str">
+        <f t="shared" ref="V4:AK21" si="2">IF(ISNUMBER(SEARCH("b",B4)),CONCATENATE(B4,": ",V$22,", ",$U4,),IF(ISNUMBER(SEARCH("w",B4)),CONCATENATE(B4,": ",V$22,", ",$U4,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 17</v>
+      </c>
+      <c r="AK4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 17</v>
+      </c>
+      <c r="AL4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 17</v>
+      </c>
+      <c r="AM4" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN4" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO4" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="5">
+        <v>16</v>
+      </c>
+      <c r="V5" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 16</v>
+      </c>
+      <c r="AK5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 16</v>
+      </c>
+      <c r="AL5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 16</v>
+      </c>
+      <c r="AM5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO5" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="5">
+        <v>15</v>
+      </c>
+      <c r="V6" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 15</v>
+      </c>
+      <c r="AK6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 15</v>
+      </c>
+      <c r="AL6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 15</v>
+      </c>
+      <c r="AM6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO6" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="5">
+        <v>14</v>
+      </c>
+      <c r="V7" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 14</v>
+      </c>
+      <c r="AK7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 14</v>
+      </c>
+      <c r="AL7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 14</v>
+      </c>
+      <c r="AM7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO7" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="5">
+        <v>13</v>
+      </c>
+      <c r="V8" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 13</v>
+      </c>
+      <c r="AK8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 13</v>
+      </c>
+      <c r="AL8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 13</v>
+      </c>
+      <c r="AM8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO8" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="5">
+        <v>12</v>
+      </c>
+      <c r="V9" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 7, 12</v>
+      </c>
+      <c r="AD9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 12</v>
+      </c>
+      <c r="AK9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 12</v>
+      </c>
+      <c r="AL9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 12</v>
+      </c>
+      <c r="AM9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO9" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="5">
+        <v>11</v>
+      </c>
+      <c r="V10" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 6, 11</v>
+      </c>
+      <c r="AC10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 7, 11</v>
+      </c>
+      <c r="AD10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b2: 8, 11</v>
+      </c>
+      <c r="AE10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 11</v>
+      </c>
+      <c r="AK10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 11</v>
+      </c>
+      <c r="AL10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 11</v>
+      </c>
+      <c r="AM10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO10" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="5">
+        <v>10</v>
+      </c>
+      <c r="V11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 6, 10</v>
+      </c>
+      <c r="AC11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 7, 10</v>
+      </c>
+      <c r="AD11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 8, 10</v>
+      </c>
+      <c r="AE11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 9, 10</v>
+      </c>
+      <c r="AF11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 10</v>
+      </c>
+      <c r="AK11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 10</v>
+      </c>
+      <c r="AL11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 10</v>
+      </c>
+      <c r="AM11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO11" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="5">
+        <v>9</v>
+      </c>
+      <c r="V12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 7, 9</v>
+      </c>
+      <c r="AD12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 8, 9</v>
+      </c>
+      <c r="AE12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 9</v>
+      </c>
+      <c r="AK12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 9</v>
+      </c>
+      <c r="AL12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 9</v>
+      </c>
+      <c r="AM12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO12" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="5">
+        <v>8</v>
+      </c>
+      <c r="V13" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 8</v>
+      </c>
+      <c r="AK13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 8</v>
+      </c>
+      <c r="AL13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 8</v>
+      </c>
+      <c r="AM13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO13" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="5">
+        <v>7</v>
+      </c>
+      <c r="V14" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 7</v>
+      </c>
+      <c r="AK14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 7</v>
+      </c>
+      <c r="AL14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 7</v>
+      </c>
+      <c r="AM14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO14" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="5">
+        <v>6</v>
+      </c>
+      <c r="V15" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 6</v>
+      </c>
+      <c r="AK15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 6</v>
+      </c>
+      <c r="AL15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 6</v>
+      </c>
+      <c r="AM15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO15" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="5">
+        <v>5</v>
+      </c>
+      <c r="V16" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 5</v>
+      </c>
+      <c r="AK16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 5</v>
+      </c>
+      <c r="AL16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 5</v>
+      </c>
+      <c r="AM16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO16" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="5">
+        <v>4</v>
+      </c>
+      <c r="V17" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 4</v>
+      </c>
+      <c r="AK17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 4</v>
+      </c>
+      <c r="AL17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 16, 4</v>
+      </c>
+      <c r="AM17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO17" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="5">
+        <v>3</v>
+      </c>
+      <c r="V18" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 14, 3</v>
+      </c>
+      <c r="AK18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 15, 3</v>
+      </c>
+      <c r="AL18" s="4" t="str">
+        <f t="shared" ref="AL18:AN21" si="3">IF(ISNUMBER(SEARCH("b",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,),IF(ISNUMBER(SEARCH("w",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,)," "))</f>
+        <v>b: 16, 3</v>
+      </c>
+      <c r="AM18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="5">
+        <v>2</v>
+      </c>
+      <c r="V19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>b: 14, 2</v>
+      </c>
+      <c r="AK19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>w: 15, 2</v>
+      </c>
+      <c r="AL19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>b: 16, 2</v>
+      </c>
+      <c r="AM19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO19" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="5">
+        <v>1</v>
+      </c>
+      <c r="V20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>b: 14, 1</v>
+      </c>
+      <c r="AK20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>w: 15, 1</v>
+      </c>
+      <c r="AL20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>b: 16, 1</v>
+      </c>
+      <c r="AM20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="5">
+        <v>0</v>
+      </c>
+      <c r="V21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>b: 14, 0</v>
+      </c>
+      <c r="AK21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>w: 15, 0</v>
+      </c>
+      <c r="AL21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>b: 16, 0</v>
+      </c>
+      <c r="AM21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" s="5" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2</v>
+      </c>
+      <c r="E22" s="5">
+        <v>3</v>
+      </c>
+      <c r="F22" s="5">
+        <v>4</v>
+      </c>
+      <c r="G22" s="5">
+        <v>5</v>
+      </c>
+      <c r="H22" s="5">
+        <v>6</v>
+      </c>
+      <c r="I22" s="5">
+        <v>7</v>
+      </c>
+      <c r="J22" s="5">
+        <v>8</v>
+      </c>
+      <c r="K22" s="5">
+        <v>9</v>
+      </c>
+      <c r="L22" s="5">
+        <v>10</v>
+      </c>
+      <c r="M22" s="5">
+        <v>11</v>
+      </c>
+      <c r="N22" s="5">
+        <v>12</v>
+      </c>
+      <c r="O22" s="5">
+        <v>13</v>
+      </c>
+      <c r="P22" s="5">
+        <v>14</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>15</v>
+      </c>
+      <c r="R22" s="5">
+        <v>16</v>
+      </c>
+      <c r="S22" s="5">
+        <v>17</v>
+      </c>
+      <c r="T22" s="5">
+        <v>18</v>
+      </c>
+      <c r="V22" s="5">
+        <v>0</v>
+      </c>
+      <c r="W22" s="5">
+        <v>1</v>
+      </c>
+      <c r="X22" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y22" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z22" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA22" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB22" s="5">
+        <v>6</v>
+      </c>
+      <c r="AC22" s="5">
+        <v>7</v>
+      </c>
+      <c r="AD22" s="5">
+        <v>8</v>
+      </c>
+      <c r="AE22" s="5">
+        <v>9</v>
+      </c>
+      <c r="AF22" s="5">
+        <v>10</v>
+      </c>
+      <c r="AG22" s="5">
+        <v>11</v>
+      </c>
+      <c r="AH22" s="5">
+        <v>12</v>
+      </c>
+      <c r="AI22" s="5">
+        <v>13</v>
+      </c>
+      <c r="AJ22" s="5">
+        <v>14</v>
+      </c>
+      <c r="AK22" s="5">
+        <v>15</v>
+      </c>
+      <c r="AL22" s="5">
+        <v>16</v>
+      </c>
+      <c r="AM22" s="5">
+        <v>17</v>
+      </c>
+      <c r="AN22" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:T2"/>
+    <mergeCell ref="V1:AN2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:T21">
+    <cfRule type="containsText" dxfId="14" priority="5" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="w">
+      <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:AN21">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="w">
+      <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:U2 A3:AN23">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="b2">
+      <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO3:AO21">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
suicide capture tests written and commented out
</commit_message>
<xml_diff>
--- a/StrategyMaster2013/src/game/go/capture_configurations.xlsx
+++ b/StrategyMaster2013/src/game/go/capture_configurations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="7" r:id="rId1"/>
@@ -14,20 +14,25 @@
     <sheet name="Complex" sheetId="9" r:id="rId5"/>
     <sheet name="MultiCapture" sheetId="10" r:id="rId6"/>
     <sheet name="MoreComplex" sheetId="11" r:id="rId7"/>
+    <sheet name="Suicides" sheetId="13" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="asdfa" localSheetId="6">#REF!</definedName>
+    <definedName name="asdfa" localSheetId="7">#REF!</definedName>
     <definedName name="asdfa">#REF!</definedName>
+    <definedName name="asdfdfd">#REF!</definedName>
     <definedName name="BoardSize" localSheetId="3">Center!#REF!</definedName>
     <definedName name="BoardSize" localSheetId="4">Complex!#REF!</definedName>
     <definedName name="BoardSize" localSheetId="1">Corners!$A$2</definedName>
     <definedName name="BoardSize" localSheetId="2">Edges!#REF!</definedName>
     <definedName name="BoardSize" localSheetId="6">MoreComplex!#REF!</definedName>
     <definedName name="BoardSize" localSheetId="5">MultiCapture!#REF!</definedName>
+    <definedName name="BoardSize" localSheetId="7">Suicides!#REF!</definedName>
     <definedName name="BoardSize" localSheetId="0">template!#REF!</definedName>
     <definedName name="BoardSize">#REF!</definedName>
     <definedName name="vb" localSheetId="6">#REF!</definedName>
     <definedName name="vb" localSheetId="5">#REF!</definedName>
+    <definedName name="vb" localSheetId="7">#REF!</definedName>
     <definedName name="vb">#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -35,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="11">
   <si>
     <t>w</t>
   </si>
@@ -193,25 +198,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="46">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -233,13 +224,6 @@
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3075,28 +3059,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="48" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="45" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="44" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="46" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="43" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="44" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="41" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="43" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5371,18 +5355,18 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="42" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="2" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="36" priority="2" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7688,28 +7672,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="34" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="36" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10031,28 +10015,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="32" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="30" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="28" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12412,28 +12396,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="26" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14743,28 +14727,28 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:AN23 A1:U2">
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14777,7 +14761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
@@ -17152,28 +17136,2343 @@
     <mergeCell ref="V1:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:T21">
-    <cfRule type="containsText" dxfId="14" priority="5" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:AN21">
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:U2 A3:AN23">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AO21">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="b2">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="b2">
+      <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AO24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" style="5"/>
+    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" customWidth="1"/>
+    <col min="21" max="21" width="4.7109375" style="6"/>
+    <col min="22" max="40" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="V1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+    </row>
+    <row r="2" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
+    </row>
+    <row r="3" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="5">
+        <v>18</v>
+      </c>
+      <c r="V3" s="4" t="str">
+        <f>IF(ISNUMBER(SEARCH("b",B3)),CONCATENATE(B3,": ",V$22,", ",$U3,),IF(ISNUMBER(SEARCH("w",B3)),CONCATENATE(B3,": ",V$22,", ",$U3,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W3" s="4" t="str">
+        <f t="shared" ref="W3:AL18" si="0">IF(ISNUMBER(SEARCH("b",C3)),CONCATENATE(C3,": ",W$22,", ",$U3,),IF(ISNUMBER(SEARCH("w",C3)),CONCATENATE(C3,": ",W$22,", ",$U3,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL3" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM3" s="4" t="str">
+        <f t="shared" ref="AM3:AN18" si="1">IF(ISNUMBER(SEARCH("b",S3)),CONCATENATE(S3,": ",AM$22,", ",$U3,),IF(ISNUMBER(SEARCH("w",S3)),CONCATENATE(S3,": ",AM$22,", ",$U3,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN3" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO3" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="5">
+        <v>17</v>
+      </c>
+      <c r="V4" s="4" t="str">
+        <f t="shared" ref="V4:AK21" si="2">IF(ISNUMBER(SEARCH("b",B4)),CONCATENATE(B4,": ",V$22,", ",$U4,),IF(ISNUMBER(SEARCH("w",B4)),CONCATENATE(B4,": ",V$22,", ",$U4,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM4" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN4" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO4" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="5">
+        <v>16</v>
+      </c>
+      <c r="V5" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO5" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="5">
+        <v>15</v>
+      </c>
+      <c r="V6" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO6" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="5">
+        <v>14</v>
+      </c>
+      <c r="V7" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO7" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="5">
+        <v>13</v>
+      </c>
+      <c r="V8" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO8" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="5">
+        <v>12</v>
+      </c>
+      <c r="V9" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO9" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="5">
+        <v>11</v>
+      </c>
+      <c r="V10" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO10" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="5">
+        <v>10</v>
+      </c>
+      <c r="V11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO11" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="5">
+        <v>9</v>
+      </c>
+      <c r="V12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO12" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="5">
+        <v>8</v>
+      </c>
+      <c r="V13" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO13" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="5">
+        <v>7</v>
+      </c>
+      <c r="V14" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO14" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="5">
+        <v>6</v>
+      </c>
+      <c r="V15" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO15" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="5">
+        <v>5</v>
+      </c>
+      <c r="V16" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 1, 5</v>
+      </c>
+      <c r="X16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO16" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="5">
+        <v>4</v>
+      </c>
+      <c r="V17" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>w: 0, 4</v>
+      </c>
+      <c r="W17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 1, 4</v>
+      </c>
+      <c r="X17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 2, 4</v>
+      </c>
+      <c r="Y17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 3, 4</v>
+      </c>
+      <c r="Z17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 4, 4</v>
+      </c>
+      <c r="AA17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO17" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="5">
+        <v>3</v>
+      </c>
+      <c r="V18" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>b: 0, 3</v>
+      </c>
+      <c r="W18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 1, 3</v>
+      </c>
+      <c r="X18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 2, 3</v>
+      </c>
+      <c r="Y18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b: 3, 3</v>
+      </c>
+      <c r="Z18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>b2: 4, 3</v>
+      </c>
+      <c r="AA18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>w: 5, 3</v>
+      </c>
+      <c r="AB18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL18" s="4" t="str">
+        <f t="shared" ref="AL18:AN21" si="3">IF(ISNUMBER(SEARCH("b",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,),IF(ISNUMBER(SEARCH("w",R18)),CONCATENATE(R18,": ",AL$22,", ",$U18,)," "))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="5">
+        <v>2</v>
+      </c>
+      <c r="V19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>b2: 0, 2</v>
+      </c>
+      <c r="W19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>w: 1, 2</v>
+      </c>
+      <c r="X19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>w: 2, 2</v>
+      </c>
+      <c r="Y19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>w: 3, 2</v>
+      </c>
+      <c r="Z19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>w: 4, 2</v>
+      </c>
+      <c r="AA19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO19" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="5">
+        <v>1</v>
+      </c>
+      <c r="V20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>w: 0, 1</v>
+      </c>
+      <c r="W20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="X20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="5">
+        <v>0</v>
+      </c>
+      <c r="V21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>b2: 0, 0</v>
+      </c>
+      <c r="W21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>w: 1, 0</v>
+      </c>
+      <c r="X21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Y21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Z21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AA21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AB21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AC21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AD21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AE21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AF21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AG21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AI21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AJ21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AK21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AL21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AM21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AN21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AO21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" s="5" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2</v>
+      </c>
+      <c r="E22" s="5">
+        <v>3</v>
+      </c>
+      <c r="F22" s="5">
+        <v>4</v>
+      </c>
+      <c r="G22" s="5">
+        <v>5</v>
+      </c>
+      <c r="H22" s="5">
+        <v>6</v>
+      </c>
+      <c r="I22" s="5">
+        <v>7</v>
+      </c>
+      <c r="J22" s="5">
+        <v>8</v>
+      </c>
+      <c r="K22" s="5">
+        <v>9</v>
+      </c>
+      <c r="L22" s="5">
+        <v>10</v>
+      </c>
+      <c r="M22" s="5">
+        <v>11</v>
+      </c>
+      <c r="N22" s="5">
+        <v>12</v>
+      </c>
+      <c r="O22" s="5">
+        <v>13</v>
+      </c>
+      <c r="P22" s="5">
+        <v>14</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>15</v>
+      </c>
+      <c r="R22" s="5">
+        <v>16</v>
+      </c>
+      <c r="S22" s="5">
+        <v>17</v>
+      </c>
+      <c r="T22" s="5">
+        <v>18</v>
+      </c>
+      <c r="V22" s="5">
+        <v>0</v>
+      </c>
+      <c r="W22" s="5">
+        <v>1</v>
+      </c>
+      <c r="X22" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y22" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z22" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA22" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB22" s="5">
+        <v>6</v>
+      </c>
+      <c r="AC22" s="5">
+        <v>7</v>
+      </c>
+      <c r="AD22" s="5">
+        <v>8</v>
+      </c>
+      <c r="AE22" s="5">
+        <v>9</v>
+      </c>
+      <c r="AF22" s="5">
+        <v>10</v>
+      </c>
+      <c r="AG22" s="5">
+        <v>11</v>
+      </c>
+      <c r="AH22" s="5">
+        <v>12</v>
+      </c>
+      <c r="AI22" s="5">
+        <v>13</v>
+      </c>
+      <c r="AJ22" s="5">
+        <v>14</v>
+      </c>
+      <c r="AK22" s="5">
+        <v>15</v>
+      </c>
+      <c r="AL22" s="5">
+        <v>16</v>
+      </c>
+      <c r="AM22" s="5">
+        <v>17</v>
+      </c>
+      <c r="AN22" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:T2"/>
+    <mergeCell ref="V1:AN2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:T21">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="w">
+      <formula>NOT(ISERROR(SEARCH("w",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:AN21">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",V3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="w">
+      <formula>NOT(ISERROR(SEARCH("w",V3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:AN23 A1:U2">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="b2">
+      <formula>NOT(ISERROR(SEARCH("b2",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO3:AO21">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="b2">
       <formula>NOT(ISERROR(SEARCH("b2",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
score keeper observing system mildly implemented
- GoScoreKeeper correctly tracks scores based on captured pieces
</commit_message>
<xml_diff>
--- a/StrategyMaster2013/src/game/go/capture_configurations.xlsx
+++ b/StrategyMaster2013/src/game/go/capture_configurations.xlsx
@@ -17170,8 +17170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="S6" workbookViewId="0">
+      <selection activeCell="AC31" sqref="AC31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18761,7 +18761,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>0</v>
@@ -18795,7 +18795,7 @@
       </c>
       <c r="W17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>b: 1, 4</v>
+        <v>b2: 1, 4</v>
       </c>
       <c r="X17" s="4" t="str">
         <f t="shared" si="0"/>

</xml_diff>